<commit_message>
Fixed Views : Add attribute required in name && margin in button Ya and No
</commit_message>
<xml_diff>
--- a/Sistem Pakar Diagnosa Malaria.xlsx
+++ b/Sistem Pakar Diagnosa Malaria.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="102">
   <si>
     <t>Demam</t>
   </si>
@@ -316,14 +317,17 @@
     <t>MERASAKAN PERASAAN SANGAT DINGIN</t>
   </si>
   <si>
-    <t>RULES</t>
+    <t>TRIAS MALARIA</t>
+  </si>
+  <si>
+    <t>RULES YANG DIPAKAI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +344,17 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -487,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -517,6 +532,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -863,7 +881,7 @@
   <dimension ref="A1:Y93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13:M13"/>
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,61 +901,61 @@
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15" t="s">
+      <c r="I1" s="18"/>
+      <c r="J1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="15"/>
+      <c r="M1" s="18"/>
       <c r="N1" s="4"/>
-      <c r="O1" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
+      <c r="O1" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
       <c r="N2" s="10"/>
       <c r="O2" s="1" t="s">
         <v>40</v>
@@ -958,20 +976,20 @@
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
       <c r="N3" s="10"/>
       <c r="P3" s="1" t="s">
         <v>97</v>
@@ -986,20 +1004,20 @@
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
       <c r="N4" s="10"/>
       <c r="P4" s="1" t="s">
         <v>42</v>
@@ -1014,20 +1032,20 @@
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
       <c r="N5" s="10"/>
       <c r="P5" s="1" t="s">
         <v>53</v>
@@ -1042,20 +1060,20 @@
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
       <c r="N6" s="10"/>
       <c r="P6" s="1" t="s">
         <v>43</v>
@@ -1070,20 +1088,20 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
       <c r="N7" s="10"/>
       <c r="P7" s="1" t="s">
         <v>47</v>
@@ -1098,20 +1116,20 @@
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="10"/>
       <c r="P8" s="1" t="s">
         <v>57</v>
@@ -1126,20 +1144,20 @@
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
       <c r="N9" s="4"/>
       <c r="P9" s="4" t="s">
         <v>58</v>
@@ -1154,20 +1172,20 @@
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="4"/>
       <c r="P10" s="4" t="s">
         <v>60</v>
@@ -1182,20 +1200,20 @@
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="4"/>
       <c r="P11" s="4" t="s">
         <v>61</v>
@@ -1210,20 +1228,20 @@
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
       <c r="N12" s="4"/>
       <c r="P12" s="1" t="s">
         <v>54</v>
@@ -1238,20 +1256,20 @@
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
       <c r="N13" s="4"/>
       <c r="P13" s="1" t="s">
         <v>98</v>
@@ -1266,20 +1284,20 @@
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
       <c r="N14" s="4"/>
       <c r="P14" s="4" t="s">
         <v>95</v>
@@ -1294,20 +1312,20 @@
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
       <c r="N15" s="9"/>
       <c r="P15" s="4" t="s">
         <v>96</v>
@@ -1322,20 +1340,20 @@
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
       <c r="N16" s="4"/>
       <c r="P16" s="4" t="s">
         <v>64</v>
@@ -1353,20 +1371,20 @@
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
       <c r="N17" s="4"/>
       <c r="O17" s="1" t="s">
         <v>45</v>
@@ -1381,20 +1399,20 @@
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
       <c r="N18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -1403,20 +1421,20 @@
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
       <c r="N19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
@@ -1425,20 +1443,20 @@
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
       <c r="N20" s="4"/>
       <c r="O20" s="1" t="s">
         <v>40</v>
@@ -1459,20 +1477,20 @@
       <c r="A21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
       <c r="N21" s="4"/>
       <c r="P21" s="1" t="s">
         <v>78</v>
@@ -1487,20 +1505,20 @@
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
       <c r="N22" s="4"/>
       <c r="P22" s="1" t="s">
         <v>79</v>
@@ -1515,20 +1533,20 @@
       <c r="A23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
       <c r="N23" s="4"/>
       <c r="P23" s="1" t="s">
         <v>42</v>
@@ -1545,22 +1563,22 @@
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="13">
+      <c r="F24" s="16">
         <v>15</v>
       </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13">
+      <c r="G24" s="16"/>
+      <c r="H24" s="16">
         <v>16</v>
       </c>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13">
+      <c r="I24" s="16"/>
+      <c r="J24" s="16">
         <v>14</v>
       </c>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13">
+      <c r="K24" s="16"/>
+      <c r="L24" s="16">
         <v>15</v>
       </c>
-      <c r="M24" s="13"/>
+      <c r="M24" s="16"/>
       <c r="N24" s="4"/>
       <c r="P24" s="1" t="s">
         <v>53</v>
@@ -2129,4 +2147,266 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G6" s="14"/>
+      <c r="H6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="14"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G15" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M17" s="15"/>
+      <c r="N17" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>